<commit_message>
HW #1 Discussion Submission
</commit_message>
<xml_diff>
--- a/Working/HW1/1D Column Model.xlsx
+++ b/Working/HW1/1D Column Model.xlsx
@@ -5,10 +5,10 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\conna\Documents\GW_Modeling\GW_Homework\Working\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\conna\Documents\GW_Modeling\GW_Homework\Working\HW1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4201ACF1-FDA4-48D8-AA31-45CE16DAF41A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0ED611E-5C7A-4CA6-9BBF-47636A730ECD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -104,7 +104,7 @@
     <definedName name="solver_ver" localSheetId="5" hidden="1">3</definedName>
     <definedName name="solver_ver" localSheetId="4" hidden="1">3</definedName>
   </definedNames>
-  <calcPr calcId="191029" iterate="1"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -5720,7 +5720,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B3:T43"/>
   <sheetViews>
-    <sheetView topLeftCell="D13" workbookViewId="0"/>
+    <sheetView topLeftCell="D30" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
@@ -6441,7 +6441,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{481C6999-B356-433A-9425-3594A7C56B0D}">
   <dimension ref="B3:W63"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView topLeftCell="M40" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="U53" sqref="U53"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
@@ -7295,7 +7297,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76653CA2-4805-495C-A3C3-5B3CFAFB6252}">
   <dimension ref="B3:W63"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P51" sqref="P51:W56"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>